<commit_message>
Minor modifications to graphs and text
</commit_message>
<xml_diff>
--- a/data/Housing infrastructure/Council tax/CTSOP1.0_SUP.xlsx
+++ b/data/Housing infrastructure/Council tax/CTSOP1.0_SUP.xlsx
@@ -21818,10 +21818,25 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f3dc68d1-c7e7-41c5-bc1e-27f8873ad3d3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="36fa22c9-99b0-4d6c-b13f-c2885a394772">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6151E689-3748-4B15-90D1-0F85518C3781}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EA9BDD9-83EF-4025-942C-D8475B1C7D70}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E01ECDA5-398F-469E-87C5-75A6CAD14724}"/>
 </file>
</xml_diff>